<commit_message>
commit av endrigner før oppload til github
</commit_message>
<xml_diff>
--- a/support_uke_24.xlsx
+++ b/support_uke_24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olal\Desktop\DIKU\prosjekt\prosjekt_DIKU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/86d7c0b08b5e5817/Studier/USN/Grunnleggende Pyton/prosjektoppgave/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086EEDD6-FC86-4C50-9462-3BEF8A47A9C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{086EEDD6-FC86-4C50-9462-3BEF8A47A9C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53ED363F-A93D-4829-94D8-026B789456EA}"/>
   <bookViews>
-    <workbookView xWindow="495" yWindow="360" windowWidth="21120" windowHeight="11895" xr2:uid="{15637531-2213-46C5-BE84-C1C04BC65914}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{15637531-2213-46C5-BE84-C1C04BC65914}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -1231,7 +1231,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1239,13 +1239,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1262,7 +1274,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1280,10 +1292,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1321,7 +1337,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1427,7 +1443,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1569,7 +1585,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1577,16 +1593,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{757D4868-2E58-4801-BECD-00865275198F}">
-  <dimension ref="A1:D218"/>
+  <dimension ref="A1:I218"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="11.42578125" style="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1595,7 +1608,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -1609,7 +1622,7 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1620,7 +1633,7 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3">
@@ -1634,7 +1647,7 @@
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1645,7 +1658,7 @@
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1656,7 +1669,7 @@
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1667,7 +1680,7 @@
       <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>15</v>
       </c>
       <c r="D7">
@@ -1681,7 +1694,7 @@
       <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1692,7 +1705,7 @@
       <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1703,7 +1716,7 @@
       <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>21</v>
       </c>
       <c r="D10">
@@ -1717,7 +1730,7 @@
       <c r="B11" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1728,7 +1741,7 @@
       <c r="B12" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1739,7 +1752,7 @@
       <c r="B13" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1750,7 +1763,7 @@
       <c r="B14" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1761,7 +1774,7 @@
       <c r="B15" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1772,7 +1785,7 @@
       <c r="B16" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1783,7 +1796,7 @@
       <c r="B17" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1794,7 +1807,7 @@
       <c r="B18" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>37</v>
       </c>
       <c r="D18">
@@ -1808,7 +1821,7 @@
       <c r="B19" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1819,7 +1832,7 @@
       <c r="B20" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1830,7 +1843,7 @@
       <c r="B21" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1841,7 +1854,7 @@
       <c r="B22" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1852,7 +1865,7 @@
       <c r="B23" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1863,7 +1876,7 @@
       <c r="B24" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1874,7 +1887,7 @@
       <c r="B25" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>37</v>
       </c>
       <c r="D25">
@@ -1888,7 +1901,7 @@
       <c r="B26" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1899,7 +1912,7 @@
       <c r="B27" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1910,7 +1923,7 @@
       <c r="B28" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1921,7 +1934,7 @@
       <c r="B29" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>21</v>
       </c>
       <c r="D29">
@@ -1935,7 +1948,7 @@
       <c r="B30" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1946,7 +1959,7 @@
       <c r="B31" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>59</v>
       </c>
       <c r="D31">
@@ -1960,7 +1973,7 @@
       <c r="B32" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1971,7 +1984,7 @@
       <c r="B33" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1982,7 +1995,7 @@
       <c r="B34" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1993,7 +2006,7 @@
       <c r="B35" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2004,7 +2017,7 @@
       <c r="B36" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2015,7 +2028,7 @@
       <c r="B37" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2026,7 +2039,7 @@
       <c r="B38" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2037,7 +2050,7 @@
       <c r="B39" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2048,7 +2061,7 @@
       <c r="B40" t="s">
         <v>74</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" t="s">
         <v>75</v>
       </c>
       <c r="D40">
@@ -2062,7 +2075,7 @@
       <c r="B41" t="s">
         <v>76</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" t="s">
         <v>77</v>
       </c>
       <c r="D41">
@@ -2076,7 +2089,7 @@
       <c r="B42" t="s">
         <v>78</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2087,7 +2100,7 @@
       <c r="B43" t="s">
         <v>79</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2098,7 +2111,7 @@
       <c r="B44" t="s">
         <v>81</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2109,7 +2122,7 @@
       <c r="B45" t="s">
         <v>83</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2120,7 +2133,7 @@
       <c r="B46" t="s">
         <v>85</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2131,7 +2144,7 @@
       <c r="B47" t="s">
         <v>87</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2142,7 +2155,7 @@
       <c r="B48" t="s">
         <v>88</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" t="s">
         <v>89</v>
       </c>
       <c r="D48">
@@ -2156,7 +2169,7 @@
       <c r="B49" t="s">
         <v>90</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" t="s">
         <v>91</v>
       </c>
       <c r="D49">
@@ -2170,7 +2183,7 @@
       <c r="B50" t="s">
         <v>92</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2181,7 +2194,7 @@
       <c r="B51" t="s">
         <v>94</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" t="s">
         <v>95</v>
       </c>
       <c r="D51">
@@ -2195,7 +2208,7 @@
       <c r="B52" t="s">
         <v>96</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2206,7 +2219,7 @@
       <c r="B53" t="s">
         <v>99</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2217,7 +2230,7 @@
       <c r="B54" t="s">
         <v>100</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2228,7 +2241,7 @@
       <c r="B55" t="s">
         <v>102</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2239,7 +2252,7 @@
       <c r="B56" t="s">
         <v>18</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2250,7 +2263,7 @@
       <c r="B57" t="s">
         <v>105</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2261,7 +2274,7 @@
       <c r="B58" t="s">
         <v>107</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2272,7 +2285,7 @@
       <c r="B59" t="s">
         <v>109</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" t="s">
         <v>110</v>
       </c>
     </row>
@@ -2283,7 +2296,7 @@
       <c r="B60" t="s">
         <v>111</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" t="s">
         <v>112</v>
       </c>
       <c r="D60">
@@ -2297,7 +2310,7 @@
       <c r="B61" t="s">
         <v>113</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" t="s">
         <v>114</v>
       </c>
       <c r="D61">
@@ -2311,7 +2324,7 @@
       <c r="B62" t="s">
         <v>115</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2322,7 +2335,7 @@
       <c r="B63" t="s">
         <v>117</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2333,7 +2346,7 @@
       <c r="B64" t="s">
         <v>119</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2344,7 +2357,7 @@
       <c r="B65" t="s">
         <v>121</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2355,7 +2368,7 @@
       <c r="B66" t="s">
         <v>123</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2366,7 +2379,7 @@
       <c r="B67" t="s">
         <v>125</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2377,7 +2390,7 @@
       <c r="B68" t="s">
         <v>127</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2388,7 +2401,7 @@
       <c r="B69" t="s">
         <v>128</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2399,7 +2412,7 @@
       <c r="B70" t="s">
         <v>130</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" t="s">
         <v>131</v>
       </c>
       <c r="D70">
@@ -2413,7 +2426,7 @@
       <c r="B71" t="s">
         <v>132</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2424,7 +2437,7 @@
       <c r="B72" t="s">
         <v>133</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" t="s">
         <v>134</v>
       </c>
       <c r="D72">
@@ -2438,7 +2451,7 @@
       <c r="B73" t="s">
         <v>135</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" t="s">
         <v>136</v>
       </c>
     </row>
@@ -2449,7 +2462,7 @@
       <c r="B74" t="s">
         <v>137</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2460,7 +2473,7 @@
       <c r="B75" t="s">
         <v>139</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2471,7 +2484,7 @@
       <c r="B76" t="s">
         <v>140</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" t="s">
         <v>141</v>
       </c>
     </row>
@@ -2482,7 +2495,7 @@
       <c r="B77" t="s">
         <v>142</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" t="s">
         <v>11</v>
       </c>
       <c r="D77">
@@ -2496,7 +2509,7 @@
       <c r="B78" t="s">
         <v>143</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2507,7 +2520,7 @@
       <c r="B79" t="s">
         <v>145</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" t="s">
         <v>146</v>
       </c>
     </row>
@@ -2518,7 +2531,7 @@
       <c r="B80" t="s">
         <v>147</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2529,7 +2542,7 @@
       <c r="B81" t="s">
         <v>149</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2540,7 +2553,7 @@
       <c r="B82" t="s">
         <v>151</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2551,7 +2564,7 @@
       <c r="B83" t="s">
         <v>153</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C83" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2562,7 +2575,7 @@
       <c r="B84" t="s">
         <v>155</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2573,7 +2586,7 @@
       <c r="B85" t="s">
         <v>157</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C85" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2584,7 +2597,7 @@
       <c r="B86" t="s">
         <v>158</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C86" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2595,7 +2608,7 @@
       <c r="B87" t="s">
         <v>160</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C87" t="s">
         <v>161</v>
       </c>
       <c r="D87">
@@ -2609,7 +2622,7 @@
       <c r="B88" t="s">
         <v>162</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C88" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2620,7 +2633,7 @@
       <c r="B89" t="s">
         <v>164</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2631,7 +2644,7 @@
       <c r="B90" t="s">
         <v>166</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C90" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2642,7 +2655,7 @@
       <c r="B91" t="s">
         <v>167</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C91" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2653,7 +2666,7 @@
       <c r="B92" t="s">
         <v>169</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C92" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2664,7 +2677,7 @@
       <c r="B93" t="s">
         <v>170</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C93" t="s">
         <v>171</v>
       </c>
       <c r="D93">
@@ -2678,7 +2691,7 @@
       <c r="B94" t="s">
         <v>172</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C94" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2689,7 +2702,7 @@
       <c r="B95" t="s">
         <v>174</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C95" t="s">
         <v>175</v>
       </c>
     </row>
@@ -2700,7 +2713,7 @@
       <c r="B96" t="s">
         <v>176</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C96" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2711,7 +2724,7 @@
       <c r="B97" t="s">
         <v>178</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C97" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2722,7 +2735,7 @@
       <c r="B98" t="s">
         <v>179</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C98" t="s">
         <v>180</v>
       </c>
     </row>
@@ -2733,7 +2746,7 @@
       <c r="B99" t="s">
         <v>181</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C99" t="s">
         <v>182</v>
       </c>
     </row>
@@ -2744,7 +2757,7 @@
       <c r="B100" t="s">
         <v>183</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C100" t="s">
         <v>184</v>
       </c>
       <c r="D100">
@@ -2758,7 +2771,7 @@
       <c r="B101" t="s">
         <v>185</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C101" t="s">
         <v>186</v>
       </c>
       <c r="D101">
@@ -2772,7 +2785,7 @@
       <c r="B102" t="s">
         <v>187</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="C102" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2783,7 +2796,7 @@
       <c r="B103" t="s">
         <v>18</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C103" t="s">
         <v>189</v>
       </c>
     </row>
@@ -2794,7 +2807,7 @@
       <c r="B104" t="s">
         <v>190</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C104" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2805,7 +2818,7 @@
       <c r="B105" t="s">
         <v>191</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C105" t="s">
         <v>192</v>
       </c>
     </row>
@@ -2816,7 +2829,7 @@
       <c r="B106" t="s">
         <v>193</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="C106" t="s">
         <v>194</v>
       </c>
     </row>
@@ -2827,7 +2840,7 @@
       <c r="B107" t="s">
         <v>195</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="C107" t="s">
         <v>196</v>
       </c>
     </row>
@@ -2838,7 +2851,7 @@
       <c r="B108" t="s">
         <v>197</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C108" t="s">
         <v>198</v>
       </c>
     </row>
@@ -2849,7 +2862,7 @@
       <c r="B109" t="s">
         <v>199</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="C109" t="s">
         <v>200</v>
       </c>
     </row>
@@ -2860,7 +2873,7 @@
       <c r="B110" t="s">
         <v>201</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="C110" t="s">
         <v>202</v>
       </c>
       <c r="D110">
@@ -2874,7 +2887,7 @@
       <c r="B111" t="s">
         <v>203</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="C111" t="s">
         <v>204</v>
       </c>
       <c r="D111">
@@ -2888,7 +2901,7 @@
       <c r="B112" t="s">
         <v>205</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="C112" t="s">
         <v>206</v>
       </c>
     </row>
@@ -2899,7 +2912,7 @@
       <c r="B113" t="s">
         <v>207</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="C113" t="s">
         <v>208</v>
       </c>
     </row>
@@ -2910,7 +2923,7 @@
       <c r="B114" t="s">
         <v>209</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="C114" t="s">
         <v>31</v>
       </c>
       <c r="D114">
@@ -2924,7 +2937,7 @@
       <c r="B115" t="s">
         <v>210</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="C115" t="s">
         <v>211</v>
       </c>
     </row>
@@ -2935,7 +2948,7 @@
       <c r="B116" t="s">
         <v>212</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="C116" t="s">
         <v>213</v>
       </c>
       <c r="D116">
@@ -2949,7 +2962,7 @@
       <c r="B117" t="s">
         <v>214</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="C117" t="s">
         <v>215</v>
       </c>
     </row>
@@ -2960,7 +2973,7 @@
       <c r="B118" t="s">
         <v>216</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="C118" t="s">
         <v>217</v>
       </c>
     </row>
@@ -2971,7 +2984,7 @@
       <c r="B119" t="s">
         <v>218</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="C119" t="s">
         <v>219</v>
       </c>
     </row>
@@ -2982,7 +2995,7 @@
       <c r="B120" t="s">
         <v>220</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="C120" t="s">
         <v>221</v>
       </c>
       <c r="D120">
@@ -2996,7 +3009,7 @@
       <c r="B121" t="s">
         <v>222</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="C121" t="s">
         <v>223</v>
       </c>
     </row>
@@ -3007,7 +3020,7 @@
       <c r="B122" t="s">
         <v>224</v>
       </c>
-      <c r="C122" s="1" t="s">
+      <c r="C122" t="s">
         <v>225</v>
       </c>
     </row>
@@ -3018,7 +3031,7 @@
       <c r="B123" t="s">
         <v>226</v>
       </c>
-      <c r="C123" s="1" t="s">
+      <c r="C123" t="s">
         <v>227</v>
       </c>
     </row>
@@ -3029,7 +3042,7 @@
       <c r="B124" t="s">
         <v>228</v>
       </c>
-      <c r="C124" s="1" t="s">
+      <c r="C124" t="s">
         <v>229</v>
       </c>
     </row>
@@ -3040,7 +3053,7 @@
       <c r="B125" t="s">
         <v>230</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="C125" t="s">
         <v>231</v>
       </c>
     </row>
@@ -3051,7 +3064,7 @@
       <c r="B126" t="s">
         <v>232</v>
       </c>
-      <c r="C126" s="1" t="s">
+      <c r="C126" t="s">
         <v>233</v>
       </c>
     </row>
@@ -3062,7 +3075,7 @@
       <c r="B127" t="s">
         <v>234</v>
       </c>
-      <c r="C127" s="1" t="s">
+      <c r="C127" t="s">
         <v>235</v>
       </c>
     </row>
@@ -3073,7 +3086,7 @@
       <c r="B128" t="s">
         <v>236</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="C128" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3084,7 +3097,7 @@
       <c r="B129" t="s">
         <v>238</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="C129" t="s">
         <v>233</v>
       </c>
       <c r="D129">
@@ -3098,7 +3111,7 @@
       <c r="B130" t="s">
         <v>239</v>
       </c>
-      <c r="C130" s="1" t="s">
+      <c r="C130" t="s">
         <v>240</v>
       </c>
     </row>
@@ -3109,7 +3122,7 @@
       <c r="B131" t="s">
         <v>241</v>
       </c>
-      <c r="C131" s="1" t="s">
+      <c r="C131" t="s">
         <v>242</v>
       </c>
       <c r="D131">
@@ -3123,7 +3136,7 @@
       <c r="B132" t="s">
         <v>243</v>
       </c>
-      <c r="C132" s="1" t="s">
+      <c r="C132" t="s">
         <v>244</v>
       </c>
     </row>
@@ -3134,7 +3147,7 @@
       <c r="B133" t="s">
         <v>245</v>
       </c>
-      <c r="C133" s="1" t="s">
+      <c r="C133" t="s">
         <v>246</v>
       </c>
     </row>
@@ -3145,7 +3158,7 @@
       <c r="B134" t="s">
         <v>247</v>
       </c>
-      <c r="C134" s="1" t="s">
+      <c r="C134" t="s">
         <v>248</v>
       </c>
     </row>
@@ -3156,7 +3169,7 @@
       <c r="B135" t="s">
         <v>249</v>
       </c>
-      <c r="C135" s="1" t="s">
+      <c r="C135" t="s">
         <v>250</v>
       </c>
     </row>
@@ -3167,7 +3180,7 @@
       <c r="B136" t="s">
         <v>251</v>
       </c>
-      <c r="C136" s="1" t="s">
+      <c r="C136" t="s">
         <v>242</v>
       </c>
     </row>
@@ -3178,7 +3191,7 @@
       <c r="B137" t="s">
         <v>252</v>
       </c>
-      <c r="C137" s="1" t="s">
+      <c r="C137" t="s">
         <v>253</v>
       </c>
     </row>
@@ -3189,7 +3202,7 @@
       <c r="B138" t="s">
         <v>254</v>
       </c>
-      <c r="C138" s="1" t="s">
+      <c r="C138" t="s">
         <v>246</v>
       </c>
     </row>
@@ -3200,7 +3213,7 @@
       <c r="B139" t="s">
         <v>255</v>
       </c>
-      <c r="C139" s="1" t="s">
+      <c r="C139" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3211,7 +3224,7 @@
       <c r="B140" t="s">
         <v>256</v>
       </c>
-      <c r="C140" s="1" t="s">
+      <c r="C140" t="s">
         <v>242</v>
       </c>
     </row>
@@ -3222,7 +3235,7 @@
       <c r="B141" t="s">
         <v>257</v>
       </c>
-      <c r="C141" s="1" t="s">
+      <c r="C141" t="s">
         <v>258</v>
       </c>
     </row>
@@ -3233,7 +3246,7 @@
       <c r="B142" t="s">
         <v>260</v>
       </c>
-      <c r="C142" s="1" t="s">
+      <c r="C142" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3244,7 +3257,7 @@
       <c r="B143" t="s">
         <v>261</v>
       </c>
-      <c r="C143" s="1" t="s">
+      <c r="C143" t="s">
         <v>262</v>
       </c>
       <c r="D143">
@@ -3258,7 +3271,7 @@
       <c r="B144" t="s">
         <v>263</v>
       </c>
-      <c r="C144" s="1" t="s">
+      <c r="C144" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3269,7 +3282,7 @@
       <c r="B145" t="s">
         <v>264</v>
       </c>
-      <c r="C145" s="1" t="s">
+      <c r="C145" t="s">
         <v>265</v>
       </c>
       <c r="D145">
@@ -3283,7 +3296,7 @@
       <c r="B146" t="s">
         <v>18</v>
       </c>
-      <c r="C146" s="1" t="s">
+      <c r="C146" t="s">
         <v>266</v>
       </c>
       <c r="D146">
@@ -3297,7 +3310,7 @@
       <c r="B147" t="s">
         <v>267</v>
       </c>
-      <c r="C147" s="1" t="s">
+      <c r="C147" t="s">
         <v>268</v>
       </c>
     </row>
@@ -3308,7 +3321,7 @@
       <c r="B148" t="s">
         <v>269</v>
       </c>
-      <c r="C148" s="1" t="s">
+      <c r="C148" t="s">
         <v>270</v>
       </c>
     </row>
@@ -3319,7 +3332,7 @@
       <c r="B149" t="s">
         <v>271</v>
       </c>
-      <c r="C149" s="1" t="s">
+      <c r="C149" t="s">
         <v>272</v>
       </c>
     </row>
@@ -3330,7 +3343,7 @@
       <c r="B150" t="s">
         <v>273</v>
       </c>
-      <c r="C150" s="1" t="s">
+      <c r="C150" t="s">
         <v>274</v>
       </c>
     </row>
@@ -3341,7 +3354,7 @@
       <c r="B151" t="s">
         <v>275</v>
       </c>
-      <c r="C151" s="1" t="s">
+      <c r="C151" t="s">
         <v>276</v>
       </c>
     </row>
@@ -3352,7 +3365,7 @@
       <c r="B152" t="s">
         <v>277</v>
       </c>
-      <c r="C152" s="1" t="s">
+      <c r="C152" t="s">
         <v>118</v>
       </c>
     </row>
@@ -3363,7 +3376,7 @@
       <c r="B153" t="s">
         <v>278</v>
       </c>
-      <c r="C153" s="1" t="s">
+      <c r="C153" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3374,7 +3387,7 @@
       <c r="B154" t="s">
         <v>279</v>
       </c>
-      <c r="C154" s="1" t="s">
+      <c r="C154" t="s">
         <v>280</v>
       </c>
       <c r="D154">
@@ -3388,7 +3401,7 @@
       <c r="B155" t="s">
         <v>281</v>
       </c>
-      <c r="C155" s="1" t="s">
+      <c r="C155" t="s">
         <v>282</v>
       </c>
       <c r="D155">
@@ -3402,7 +3415,7 @@
       <c r="B156" t="s">
         <v>283</v>
       </c>
-      <c r="C156" s="1" t="s">
+      <c r="C156" t="s">
         <v>284</v>
       </c>
       <c r="D156">
@@ -3416,7 +3429,7 @@
       <c r="B157" t="s">
         <v>285</v>
       </c>
-      <c r="C157" s="1" t="s">
+      <c r="C157" t="s">
         <v>286</v>
       </c>
     </row>
@@ -3427,7 +3440,7 @@
       <c r="B158" t="s">
         <v>287</v>
       </c>
-      <c r="C158" s="1" t="s">
+      <c r="C158" t="s">
         <v>288</v>
       </c>
     </row>
@@ -3438,7 +3451,7 @@
       <c r="B159" t="s">
         <v>289</v>
       </c>
-      <c r="C159" s="1" t="s">
+      <c r="C159" t="s">
         <v>290</v>
       </c>
     </row>
@@ -3449,7 +3462,7 @@
       <c r="B160" t="s">
         <v>291</v>
       </c>
-      <c r="C160" s="1" t="s">
+      <c r="C160" t="s">
         <v>292</v>
       </c>
     </row>
@@ -3460,7 +3473,7 @@
       <c r="B161" t="s">
         <v>293</v>
       </c>
-      <c r="C161" s="1" t="s">
+      <c r="C161" t="s">
         <v>294</v>
       </c>
     </row>
@@ -3471,7 +3484,7 @@
       <c r="B162" t="s">
         <v>295</v>
       </c>
-      <c r="C162" s="1" t="s">
+      <c r="C162" t="s">
         <v>296</v>
       </c>
     </row>
@@ -3482,7 +3495,7 @@
       <c r="B163" t="s">
         <v>297</v>
       </c>
-      <c r="C163" s="1" t="s">
+      <c r="C163" t="s">
         <v>298</v>
       </c>
       <c r="D163">
@@ -3496,7 +3509,7 @@
       <c r="B164" t="s">
         <v>299</v>
       </c>
-      <c r="C164" s="1" t="s">
+      <c r="C164" t="s">
         <v>300</v>
       </c>
     </row>
@@ -3507,7 +3520,7 @@
       <c r="B165" t="s">
         <v>301</v>
       </c>
-      <c r="C165" s="1" t="s">
+      <c r="C165" t="s">
         <v>302</v>
       </c>
       <c r="D165">
@@ -3521,7 +3534,7 @@
       <c r="B166" t="s">
         <v>303</v>
       </c>
-      <c r="C166" s="1" t="s">
+      <c r="C166" t="s">
         <v>304</v>
       </c>
     </row>
@@ -3532,7 +3545,7 @@
       <c r="B167" t="s">
         <v>305</v>
       </c>
-      <c r="C167" s="1" t="s">
+      <c r="C167" t="s">
         <v>306</v>
       </c>
     </row>
@@ -3543,7 +3556,7 @@
       <c r="B168" t="s">
         <v>307</v>
       </c>
-      <c r="C168" s="1" t="s">
+      <c r="C168" t="s">
         <v>308</v>
       </c>
     </row>
@@ -3554,7 +3567,7 @@
       <c r="B169" t="s">
         <v>309</v>
       </c>
-      <c r="C169" s="1" t="s">
+      <c r="C169" t="s">
         <v>310</v>
       </c>
     </row>
@@ -3565,7 +3578,7 @@
       <c r="B170" t="s">
         <v>311</v>
       </c>
-      <c r="C170" s="1" t="s">
+      <c r="C170" t="s">
         <v>304</v>
       </c>
     </row>
@@ -3576,7 +3589,7 @@
       <c r="B171" t="s">
         <v>312</v>
       </c>
-      <c r="C171" s="1" t="s">
+      <c r="C171" t="s">
         <v>313</v>
       </c>
     </row>
@@ -3587,7 +3600,7 @@
       <c r="B172" t="s">
         <v>314</v>
       </c>
-      <c r="C172" s="1" t="s">
+      <c r="C172" t="s">
         <v>315</v>
       </c>
       <c r="D172">
@@ -3601,7 +3614,7 @@
       <c r="B173" t="s">
         <v>316</v>
       </c>
-      <c r="C173" s="1" t="s">
+      <c r="C173" t="s">
         <v>317</v>
       </c>
     </row>
@@ -3612,7 +3625,7 @@
       <c r="B174" t="s">
         <v>318</v>
       </c>
-      <c r="C174" s="1" t="s">
+      <c r="C174" t="s">
         <v>319</v>
       </c>
     </row>
@@ -3623,7 +3636,7 @@
       <c r="B175" t="s">
         <v>320</v>
       </c>
-      <c r="C175" s="1" t="s">
+      <c r="C175" t="s">
         <v>317</v>
       </c>
     </row>
@@ -3634,7 +3647,7 @@
       <c r="B176" t="s">
         <v>321</v>
       </c>
-      <c r="C176" s="1" t="s">
+      <c r="C176" t="s">
         <v>322</v>
       </c>
     </row>
@@ -3645,7 +3658,7 @@
       <c r="B177" t="s">
         <v>324</v>
       </c>
-      <c r="C177" s="1" t="s">
+      <c r="C177" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3656,7 +3669,7 @@
       <c r="B178" t="s">
         <v>325</v>
       </c>
-      <c r="C178" s="1" t="s">
+      <c r="C178" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3667,7 +3680,7 @@
       <c r="B179" t="s">
         <v>18</v>
       </c>
-      <c r="C179" s="1" t="s">
+      <c r="C179" t="s">
         <v>326</v>
       </c>
     </row>
@@ -3678,7 +3691,7 @@
       <c r="B180" t="s">
         <v>327</v>
       </c>
-      <c r="C180" s="1" t="s">
+      <c r="C180" t="s">
         <v>328</v>
       </c>
     </row>
@@ -3689,7 +3702,7 @@
       <c r="B181" t="s">
         <v>329</v>
       </c>
-      <c r="C181" s="1" t="s">
+      <c r="C181" t="s">
         <v>317</v>
       </c>
     </row>
@@ -3700,7 +3713,7 @@
       <c r="B182" t="s">
         <v>330</v>
       </c>
-      <c r="C182" s="1" t="s">
+      <c r="C182" t="s">
         <v>331</v>
       </c>
     </row>
@@ -3711,7 +3724,7 @@
       <c r="B183" t="s">
         <v>332</v>
       </c>
-      <c r="C183" s="1" t="s">
+      <c r="C183" t="s">
         <v>317</v>
       </c>
       <c r="D183">
@@ -3725,7 +3738,7 @@
       <c r="B184" t="s">
         <v>333</v>
       </c>
-      <c r="C184" s="1" t="s">
+      <c r="C184" t="s">
         <v>334</v>
       </c>
       <c r="D184">
@@ -3739,7 +3752,7 @@
       <c r="B185" t="s">
         <v>335</v>
       </c>
-      <c r="C185" s="1" t="s">
+      <c r="C185" t="s">
         <v>336</v>
       </c>
     </row>
@@ -3750,7 +3763,7 @@
       <c r="B186" t="s">
         <v>337</v>
       </c>
-      <c r="C186" s="1" t="s">
+      <c r="C186" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3761,7 +3774,7 @@
       <c r="B187" t="s">
         <v>338</v>
       </c>
-      <c r="C187" s="1" t="s">
+      <c r="C187" t="s">
         <v>339</v>
       </c>
     </row>
@@ -3772,7 +3785,7 @@
       <c r="B188" t="s">
         <v>340</v>
       </c>
-      <c r="C188" s="1" t="s">
+      <c r="C188" t="s">
         <v>336</v>
       </c>
     </row>
@@ -3783,7 +3796,7 @@
       <c r="B189" t="s">
         <v>341</v>
       </c>
-      <c r="C189" s="1" t="s">
+      <c r="C189" t="s">
         <v>342</v>
       </c>
     </row>
@@ -3794,7 +3807,7 @@
       <c r="B190" t="s">
         <v>343</v>
       </c>
-      <c r="C190" s="1" t="s">
+      <c r="C190" t="s">
         <v>344</v>
       </c>
     </row>
@@ -3805,7 +3818,7 @@
       <c r="B191" t="s">
         <v>345</v>
       </c>
-      <c r="C191" s="1" t="s">
+      <c r="C191" t="s">
         <v>346</v>
       </c>
     </row>
@@ -3816,186 +3829,187 @@
       <c r="B192" t="s">
         <v>137</v>
       </c>
-      <c r="C192" s="1" t="s">
+      <c r="C192" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>323</v>
       </c>
       <c r="B193" t="s">
         <v>347</v>
       </c>
-      <c r="C193" s="1" t="s">
+      <c r="C193" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>323</v>
       </c>
       <c r="B194" t="s">
         <v>349</v>
       </c>
-      <c r="C194" s="1" t="s">
+      <c r="C194" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I194" s="1"/>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>323</v>
       </c>
       <c r="B195" t="s">
         <v>351</v>
       </c>
-      <c r="C195" s="1" t="s">
+      <c r="C195" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>323</v>
       </c>
       <c r="B196" t="s">
         <v>353</v>
       </c>
-      <c r="C196" s="1" t="s">
+      <c r="C196" t="s">
         <v>354</v>
       </c>
       <c r="D196">
         <v>10</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>323</v>
       </c>
       <c r="B197" t="s">
         <v>355</v>
       </c>
-      <c r="C197" s="1" t="s">
+      <c r="C197" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>323</v>
       </c>
       <c r="B198" t="s">
         <v>357</v>
       </c>
-      <c r="C198" s="1" t="s">
+      <c r="C198" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>323</v>
       </c>
       <c r="B199" t="s">
         <v>359</v>
       </c>
-      <c r="C199" s="1" t="s">
+      <c r="C199" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>323</v>
       </c>
       <c r="B200" t="s">
         <v>360</v>
       </c>
-      <c r="C200" s="1" t="s">
+      <c r="C200" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>323</v>
       </c>
       <c r="B201" t="s">
         <v>362</v>
       </c>
-      <c r="C201" s="1" t="s">
+      <c r="C201" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>323</v>
       </c>
       <c r="B202" t="s">
         <v>364</v>
       </c>
-      <c r="C202" s="1" t="s">
+      <c r="C202" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>323</v>
       </c>
       <c r="B203" t="s">
         <v>366</v>
       </c>
-      <c r="C203" s="1" t="s">
+      <c r="C203" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>323</v>
       </c>
       <c r="B204" t="s">
         <v>368</v>
       </c>
-      <c r="C204" s="1" t="s">
+      <c r="C204" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>323</v>
       </c>
       <c r="B205" t="s">
         <v>370</v>
       </c>
-      <c r="C205" s="1" t="s">
+      <c r="C205" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>323</v>
       </c>
       <c r="B206" t="s">
         <v>372</v>
       </c>
-      <c r="C206" s="1" t="s">
+      <c r="C206" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>323</v>
       </c>
       <c r="B207" t="s">
         <v>374</v>
       </c>
-      <c r="C207" s="1" t="s">
+      <c r="C207" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>323</v>
       </c>
       <c r="B208" t="s">
         <v>376</v>
       </c>
-      <c r="C208" s="1" t="s">
+      <c r="C208" t="s">
         <v>377</v>
       </c>
     </row>
@@ -4006,7 +4020,7 @@
       <c r="B209" t="s">
         <v>378</v>
       </c>
-      <c r="C209" s="1" t="s">
+      <c r="C209" t="s">
         <v>379</v>
       </c>
     </row>
@@ -4017,7 +4031,7 @@
       <c r="B210" t="s">
         <v>380</v>
       </c>
-      <c r="C210" s="1" t="s">
+      <c r="C210" t="s">
         <v>381</v>
       </c>
       <c r="D210">
@@ -4031,7 +4045,7 @@
       <c r="B211" t="s">
         <v>382</v>
       </c>
-      <c r="C211" s="1" t="s">
+      <c r="C211" t="s">
         <v>383</v>
       </c>
       <c r="D211">
@@ -4045,7 +4059,7 @@
       <c r="B212" t="s">
         <v>384</v>
       </c>
-      <c r="C212" s="1" t="s">
+      <c r="C212" t="s">
         <v>385</v>
       </c>
     </row>
@@ -4056,7 +4070,7 @@
       <c r="B213" t="s">
         <v>386</v>
       </c>
-      <c r="C213" s="1" t="s">
+      <c r="C213" t="s">
         <v>387</v>
       </c>
     </row>
@@ -4067,7 +4081,7 @@
       <c r="B214" t="s">
         <v>388</v>
       </c>
-      <c r="C214" s="1" t="s">
+      <c r="C214" t="s">
         <v>389</v>
       </c>
     </row>
@@ -4078,7 +4092,7 @@
       <c r="B215" t="s">
         <v>390</v>
       </c>
-      <c r="C215" s="1" t="s">
+      <c r="C215" t="s">
         <v>29</v>
       </c>
     </row>
@@ -4089,7 +4103,7 @@
       <c r="B216" t="s">
         <v>391</v>
       </c>
-      <c r="C216" s="1" t="s">
+      <c r="C216" t="s">
         <v>392</v>
       </c>
     </row>
@@ -4100,7 +4114,7 @@
       <c r="B217" t="s">
         <v>393</v>
       </c>
-      <c r="C217" s="1" t="s">
+      <c r="C217" t="s">
         <v>394</v>
       </c>
     </row>
@@ -4111,7 +4125,7 @@
       <c r="B218" t="s">
         <v>395</v>
       </c>
-      <c r="C218" s="1" t="s">
+      <c r="C218" t="s">
         <v>396</v>
       </c>
       <c r="D218">
@@ -4119,6 +4133,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>